<commit_message>
Changes to accommodate remote clocking (using CLK_FIN only, FTSW version not yet implemented).  Added command interpreter ROM file to project so that you don't have to assemble it yourself (picoblaze processor still must be downloaded [for free] from Xilinx.  Fixed a bug in ROI parser that would lock the system up if the first and last allowed addresses were identical.
</commit_message>
<xml_diff>
--- a/SCROD-boardstack/new_daq_interface/contrib/register_map.xlsx
+++ b/SCROD-boardstack/new_daq_interface/contrib/register_map.xlsx
@@ -12,7 +12,6 @@
     <sheet name="DAC Mappings (IRS2 DC RevB2)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -734,8 +733,8 @@
   <dimension ref="A1:G258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G168" sqref="G168"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6077,7 +6076,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B261" sqref="B261"/>
+      <selection pane="bottomLeft" activeCell="F261" sqref="F261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>